<commit_message>
admin user and profile view implemented
</commit_message>
<xml_diff>
--- a/uploads/subscriberInfo.xlsx
+++ b/uploads/subscriberInfo.xlsx
@@ -50,14 +50,14 @@
     <t>group</t>
   </si>
   <si>
-    <t>test</t>
+    <t>Test1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -92,6 +92,12 @@
     <font>
       <sz val="10"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -126,7 +132,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -140,6 +146,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -454,7 +461,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -484,9 +491,9 @@
         <v>9902224895</v>
       </c>
       <c r="C2">
-        <v>13</v>
-      </c>
-      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>8</v>
       </c>
     </row>
@@ -498,9 +505,9 @@
         <v>9886498456</v>
       </c>
       <c r="C3">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="7" t="s">
         <v>8</v>
       </c>
     </row>
@@ -512,9 +519,9 @@
         <v>9141690022</v>
       </c>
       <c r="C4">
-        <v>15</v>
-      </c>
-      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>8</v>
       </c>
     </row>
@@ -526,9 +533,9 @@
         <v>7795623768</v>
       </c>
       <c r="C5">
-        <v>16</v>
-      </c>
-      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="7" t="s">
         <v>8</v>
       </c>
     </row>
@@ -554,5 +561,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
login-signup fixed, logout button implemented
</commit_message>
<xml_diff>
--- a/uploads/subscriberInfo.xlsx
+++ b/uploads/subscriberInfo.xlsx
@@ -50,7 +50,7 @@
     <t>group</t>
   </si>
   <si>
-    <t>Test1</t>
+    <t>ZC-001A</t>
   </si>
 </sst>
 </file>
@@ -461,7 +461,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D3" sqref="D3:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
changes after first demo
</commit_message>
<xml_diff>
--- a/uploads/subscriberInfo.xlsx
+++ b/uploads/subscriberInfo.xlsx
@@ -50,7 +50,7 @@
     <t>group</t>
   </si>
   <si>
-    <t>ZC-001A</t>
+    <t>Test</t>
   </si>
 </sst>
 </file>
@@ -491,7 +491,7 @@
         <v>9902224895</v>
       </c>
       <c r="C2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
check of number of sucribers before adding subscribers to the group implemented
</commit_message>
<xml_diff>
--- a/uploads/subscriberInfo.xlsx
+++ b/uploads/subscriberInfo.xlsx
@@ -50,7 +50,7 @@
     <t>group</t>
   </si>
   <si>
-    <t>Test</t>
+    <t>ZC-001A</t>
   </si>
 </sst>
 </file>
@@ -461,7 +461,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:D5"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -491,7 +491,7 @@
         <v>9902224895</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>8</v>

</xml_diff>